<commit_message>
added nginx and 2-th week with questions
</commit_message>
<xml_diff>
--- a/exel_tracker/devops_learning_tracker_complete.xlsx
+++ b/exel_tracker/devops_learning_tracker_complete.xlsx
@@ -634,7 +634,7 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -769,6 +769,7 @@
       <c r="D9" s="5" t="s">
         <v>16</v>
       </c>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="n">
@@ -781,6 +782,7 @@
       <c r="D10" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="n">

</xml_diff>